<commit_message>
Pivot with a lambda may be appropriate
</commit_message>
<xml_diff>
--- a/StrategicPlanningFunction.xlsx
+++ b/StrategicPlanningFunction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C051D511-557A-4EED-8189-D5841C6684FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{133C7815-4487-4B96-8999-521E20C99BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
   <si>
     <t>FROM:</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Feature A</t>
   </si>
 </sst>
 </file>
@@ -278,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,6 +330,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -371,7 +386,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -381,6 +396,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -1230,8 +1254,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3662C2EC-8CA9-426E-B125-1F5650A90F36}" name="_tExample" displayName="_tExample" ref="C6:F15" totalsRowShown="0">
-  <autoFilter ref="C6:F15" xr:uid="{3662C2EC-8CA9-426E-B125-1F5650A90F36}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3662C2EC-8CA9-426E-B125-1F5650A90F36}" name="_tExample" displayName="_tExample" ref="C6:F16" totalsRowShown="0">
+  <autoFilter ref="C6:F16" xr:uid="{3662C2EC-8CA9-426E-B125-1F5650A90F36}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B3734F07-0DAE-4E29-B78F-71F3D57F3D1A}" name="Strategy"/>
     <tableColumn id="2" xr3:uid="{D5EE77A1-1EE5-4D2B-9E0C-F9245A7BD142}" name="Program"/>
@@ -1445,10 +1469,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="C6:L15"/>
+  <dimension ref="C2:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I2" sqref="I2:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1457,9 +1481,56 @@
     <col min="4" max="4" width="9.88671875" customWidth="1"/>
     <col min="5" max="5" width="10.109375" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I2" t="str" cm="1">
+        <f t="array" ref="I2:K10">_xlfn.DROP(_xlfn._xlws.FILTER(_tExample[],_tExample[Critical]="x"),,-1)</f>
+        <v>Mark</v>
+      </c>
+      <c r="J2" t="str">
+        <v>A</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Feature 1</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I3" t="str">
+        <v>Mark</v>
+      </c>
+      <c r="J3" t="str">
+        <v>A</v>
+      </c>
+      <c r="K3" t="str">
+        <v>Feature 2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I4" t="str">
+        <v>Mark</v>
+      </c>
+      <c r="J4" t="str">
+        <v>A</v>
+      </c>
+      <c r="K4" t="str">
+        <v>Feature A</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I5" t="str">
+        <v>Mark</v>
+      </c>
+      <c r="J5" t="str">
+        <v>C</v>
+      </c>
+      <c r="K5" t="str">
+        <v>Feature 3</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>21</v>
       </c>
@@ -1472,21 +1543,17 @@
       <c r="F6" t="s">
         <v>37</v>
       </c>
-      <c r="I6" t="str" cm="1">
-        <f t="array" ref="I6:L12">_xlfn._xlws.FILTER(_tExample[],_tExample[Critical]="x")</f>
+      <c r="I6" t="str">
         <v>Mark</v>
       </c>
       <c r="J6" t="str">
-        <v>A</v>
+        <v>D</v>
       </c>
       <c r="K6" t="str">
-        <v>Feature 1</v>
-      </c>
-      <c r="L6" t="str">
-        <v>x</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+        <v>Feature 4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>22</v>
       </c>
@@ -1500,24 +1567,21 @@
         <v>38</v>
       </c>
       <c r="I7" t="str">
-        <v>Mark</v>
+        <v>Craig</v>
       </c>
       <c r="J7" t="str">
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="K7" t="str">
-        <v>Feature 2</v>
-      </c>
-      <c r="L7" t="str">
-        <v>x</v>
-      </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+        <v>Feature 5</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -1526,27 +1590,24 @@
         <v>38</v>
       </c>
       <c r="I8" t="str">
-        <v>Mark</v>
+        <v>Craig</v>
       </c>
       <c r="J8" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="K8" t="str">
-        <v>Feature 3</v>
-      </c>
-      <c r="L8" t="str">
-        <v>x</v>
-      </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+        <v>Feature 6</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
         <v>38</v>
@@ -1555,128 +1616,184 @@
         <v>Craig</v>
       </c>
       <c r="J9" t="str">
-        <v>A</v>
+        <v>D</v>
       </c>
       <c r="K9" t="str">
-        <v>Feature 5</v>
-      </c>
-      <c r="L9" t="str">
-        <v>x</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+        <v>Feature 8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
       </c>
       <c r="I10" t="str">
         <v>Craig</v>
       </c>
       <c r="J10" t="str">
-        <v>B</v>
+        <v>E</v>
       </c>
       <c r="K10" t="str">
-        <v>Feature 6</v>
-      </c>
-      <c r="L10" t="str">
-        <v>x</v>
-      </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+        <v>Feature 9</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
         <v>38</v>
       </c>
-      <c r="I11" t="str">
-        <v>Craig</v>
-      </c>
-      <c r="J11" t="str">
-        <v>D</v>
-      </c>
-      <c r="K11" t="str">
-        <v>Feature 8</v>
-      </c>
-      <c r="L11" t="str">
-        <v>x</v>
-      </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
         <v>38</v>
       </c>
-      <c r="I12" t="str">
-        <v>Craig</v>
-      </c>
-      <c r="J12" t="str">
-        <v>E</v>
-      </c>
-      <c r="K12" t="str">
-        <v>Feature 9</v>
-      </c>
-      <c r="L12" t="str">
-        <v>x</v>
-      </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="9:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="11" t="str" cm="1">
+        <f t="array" ref="I21:M23">_xlfn.PIVOTBY(I2:I9,J2:J9,K2:K9,_xlfn.LAMBDA(_xlpm.x,_xlfn.TEXTJOIN(CHAR(10),FALSE,_xlpm.x)),,0,,0)</f>
+        <v/>
+      </c>
+      <c r="J21" s="11" t="str">
+        <v>A</v>
+      </c>
+      <c r="K21" s="11" t="str">
+        <v>B</v>
+      </c>
+      <c r="L21" s="11" t="str">
+        <v>C</v>
+      </c>
+      <c r="M21" s="11" t="str">
+        <v>D</v>
+      </c>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+    </row>
+    <row r="22" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I22" s="10" t="str">
+        <v>Craig</v>
+      </c>
+      <c r="J22" s="10" t="str">
+        <v>Feature 5</v>
+      </c>
+      <c r="K22" s="10" t="str">
+        <v>Feature 6</v>
+      </c>
+      <c r="L22" s="10" t="str">
+        <v/>
+      </c>
+      <c r="M22" s="10" t="str">
+        <v>Feature 8</v>
+      </c>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+    </row>
+    <row r="23" spans="9:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="I23" s="10" t="str">
+        <v>Mark</v>
+      </c>
+      <c r="J23" s="10" t="str">
+        <v>Feature 1
+Feature 2
+Feature A</v>
+      </c>
+      <c r="K23" s="10" t="str">
+        <v/>
+      </c>
+      <c r="L23" s="10" t="str">
+        <v>Feature 3</v>
+      </c>
+      <c r="M23" s="10" t="str">
+        <v>Feature 4</v>
+      </c>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+    </row>
+    <row r="24" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J5:J8">

</xml_diff>

<commit_message>
Groupby was not productive
</commit_message>
<xml_diff>
--- a/StrategicPlanningFunction.xlsx
+++ b/StrategicPlanningFunction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{133C7815-4487-4B96-8999-521E20C99BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{644C43B3-271F-4A7B-B5A9-80591B86875D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -1464,6 +1464,29 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{AA69C28E-4BF0-4F06-BF5C-F9ACE4586ACB}">
+  <we:reference id="wa200006821" version="1.0.0.1" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200006821" version="1.0.0.1" store="WA200006821" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="filterText" value="null"/>
+    <we:property name="isFirstTime" value="false"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1">
@@ -1472,7 +1495,7 @@
   <dimension ref="C2:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:K10"/>
+      <selection activeCell="I21" sqref="I21:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1616,7 +1639,7 @@
         <v>Craig</v>
       </c>
       <c r="J9" t="str">
-        <v>D</v>
+        <v>B</v>
       </c>
       <c r="K9" t="str">
         <v>Feature 8</v>
@@ -1703,7 +1726,7 @@
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
         <v>33</v>
@@ -1746,7 +1769,7 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
     </row>
-    <row r="22" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:15" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I22" s="10" t="str">
         <v>Craig</v>
       </c>
@@ -1754,13 +1777,14 @@
         <v>Feature 5</v>
       </c>
       <c r="K22" s="10" t="str">
-        <v>Feature 6</v>
+        <v>Feature 6
+Feature 8</v>
       </c>
       <c r="L22" s="10" t="str">
         <v/>
       </c>
       <c r="M22" s="10" t="str">
-        <v>Feature 8</v>
+        <v/>
       </c>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>

</xml_diff>

<commit_message>
I got a pretty good start on a single function
</commit_message>
<xml_diff>
--- a/StrategicPlanningFunction.xlsx
+++ b/StrategicPlanningFunction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{644C43B3-271F-4A7B-B5A9-80591B86875D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB31BE01-9BFC-463F-B2BC-696E71DA1777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -18,11 +18,12 @@
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_exclude">Report!$M$3:$M$4</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,6 +36,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -64,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>FROM:</t>
   </si>
@@ -184,6 +187,21 @@
   </si>
   <si>
     <t>Feature A</t>
+  </si>
+  <si>
+    <t>Boff</t>
+  </si>
+  <si>
+    <t>Biff</t>
+  </si>
+  <si>
+    <t>Exclude</t>
+  </si>
+  <si>
+    <t>Feature 10</t>
+  </si>
+  <si>
+    <t>Feature 11</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1182,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1254,8 +1272,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3662C2EC-8CA9-426E-B125-1F5650A90F36}" name="_tExample" displayName="_tExample" ref="C6:F16" totalsRowShown="0">
-  <autoFilter ref="C6:F16" xr:uid="{3662C2EC-8CA9-426E-B125-1F5650A90F36}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3662C2EC-8CA9-426E-B125-1F5650A90F36}" name="_tExample" displayName="_tExample" ref="C6:F18" totalsRowShown="0">
+  <autoFilter ref="C6:F18" xr:uid="{3662C2EC-8CA9-426E-B125-1F5650A90F36}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B3734F07-0DAE-4E29-B78F-71F3D57F3D1A}" name="Strategy"/>
     <tableColumn id="2" xr3:uid="{D5EE77A1-1EE5-4D2B-9E0C-F9245A7BD142}" name="Program"/>
@@ -1492,10 +1510,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="C2:O24"/>
+  <dimension ref="C2:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:M23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1506,11 +1524,16 @@
     <col min="6" max="6" width="10.88671875" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" customWidth="1"/>
+    <col min="17" max="17" width="21" customWidth="1"/>
+    <col min="18" max="18" width="12.109375" customWidth="1"/>
+    <col min="19" max="19" width="13.5546875" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
       <c r="I2" t="str" cm="1">
-        <f t="array" ref="I2:K10">_xlfn.DROP(_xlfn._xlws.FILTER(_tExample[],_tExample[Critical]="x"),,-1)</f>
+        <f t="array" ref="I2:K12">_xlfn.DROP(_xlfn._xlws.FILTER(_tExample[],_tExample[Critical]="x"),,-1)</f>
         <v>Mark</v>
       </c>
       <c r="J2" t="str">
@@ -1519,8 +1542,11 @@
       <c r="K2" t="str">
         <v>Feature 1</v>
       </c>
-    </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
       <c r="I3" t="str">
         <v>Mark</v>
       </c>
@@ -1530,8 +1556,11 @@
       <c r="K3" t="str">
         <v>Feature 2</v>
       </c>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="I4" t="str">
         <v>Mark</v>
       </c>
@@ -1541,8 +1570,11 @@
       <c r="K4" t="str">
         <v>Feature A</v>
       </c>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
       <c r="I5" t="str">
         <v>Mark</v>
       </c>
@@ -1553,7 +1585,7 @@
         <v>Feature 3</v>
       </c>
     </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>21</v>
       </c>
@@ -1576,7 +1608,7 @@
         <v>Feature 4</v>
       </c>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>22</v>
       </c>
@@ -1599,7 +1631,7 @@
         <v>Feature 5</v>
       </c>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>22</v>
       </c>
@@ -1622,7 +1654,7 @@
         <v>Feature 6</v>
       </c>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>22</v>
       </c>
@@ -1645,7 +1677,7 @@
         <v>Feature 8</v>
       </c>
     </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>22</v>
       </c>
@@ -1668,7 +1700,7 @@
         <v>Feature 9</v>
       </c>
     </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>22</v>
       </c>
@@ -1681,8 +1713,17 @@
       <c r="F11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I11" t="str">
+        <v>Boff</v>
+      </c>
+      <c r="J11" t="str">
+        <v>A</v>
+      </c>
+      <c r="K11" t="str">
+        <v>Feature 10</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>23</v>
       </c>
@@ -1695,8 +1736,17 @@
       <c r="F12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I12" t="str">
+        <v>Biff</v>
+      </c>
+      <c r="J12" t="str">
+        <v>B</v>
+      </c>
+      <c r="K12" t="str">
+        <v>Feature 11</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>23</v>
       </c>
@@ -1710,7 +1760,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>23</v>
       </c>
@@ -1721,7 +1771,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>23</v>
       </c>
@@ -1735,7 +1785,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>23</v>
       </c>
@@ -1749,7 +1799,35 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="9:15" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I21" s="11" t="str" cm="1">
         <f t="array" ref="I21:M23">_xlfn.PIVOTBY(I2:I9,J2:J9,K2:K9,_xlfn.LAMBDA(_xlpm.x,_xlfn.TEXTJOIN(CHAR(10),FALSE,_xlpm.x)),,0,,0)</f>
         <v/>
@@ -1767,9 +1845,33 @@
         <v>D</v>
       </c>
       <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-    </row>
-    <row r="22" spans="9:15" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O21" s="11" t="str" cm="1">
+        <f t="array" ref="O21:T23">_xlfn.LET(
+_xlpm.u,  _xlfn.UNIQUE(_xlfn._xlws.FILTER(_tExample[Strategy],_tExample[Critical]="x")),
+_xlpm.ue, _xlfn._xlws.FILTER(_xlpm.u, ISNA(MATCH(_xlpm.u, _exclude, 0))),
+_xlpm.z, _xlfn.HSTACK(C7:C18,D7:D18,E7:E18),
+_xlpm.q, _xlfn.DROP(_xlfn.REDUCE("",_xlpm.ue,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn._xlws.FILTER(_xlpm.z,_xlfn.TAKE(_xlpm.z,,1)=_xlpm.v)))),1),
+_xlfn.PIVOTBY(_xlfn.TAKE(_xlpm.q,,1),_xlfn.CHOOSECOLS(_xlpm.q,2),_xlfn.TAKE(_xlpm.q,,-1),_xlfn.LAMBDA(_xlpm.x,_xlfn.TEXTJOIN(CHAR(10),FALSE,_xlpm.x)),,0,,0)
+)</f>
+        <v/>
+      </c>
+      <c r="P21" s="11" t="str">
+        <v>A</v>
+      </c>
+      <c r="Q21" s="11" t="str">
+        <v>B</v>
+      </c>
+      <c r="R21" s="11" t="str">
+        <v>C</v>
+      </c>
+      <c r="S21" s="11" t="str">
+        <v>D</v>
+      </c>
+      <c r="T21" s="11" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="22" spans="3:20" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I22" s="10" t="str">
         <v>Craig</v>
       </c>
@@ -1787,9 +1889,27 @@
         <v/>
       </c>
       <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-    </row>
-    <row r="23" spans="9:15" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="O22" s="10" t="str">
+        <v>Craig</v>
+      </c>
+      <c r="P22" s="10" t="str">
+        <v>Feature 5</v>
+      </c>
+      <c r="Q22" s="10" t="str">
+        <v>Feature 6
+Feature 8</v>
+      </c>
+      <c r="R22" s="10" t="str">
+        <v>Feature 7</v>
+      </c>
+      <c r="S22" s="10" t="str">
+        <v/>
+      </c>
+      <c r="T22" s="10" t="str">
+        <v>Feature 9</v>
+      </c>
+    </row>
+    <row r="23" spans="3:20" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I23" s="10" t="str">
         <v>Mark</v>
       </c>
@@ -1808,9 +1928,28 @@
         <v>Feature 4</v>
       </c>
       <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-    </row>
-    <row r="24" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="O23" s="10" t="str">
+        <v>Mark</v>
+      </c>
+      <c r="P23" s="10" t="str">
+        <v>Feature 1
+Feature 2
+Feature A</v>
+      </c>
+      <c r="Q23" s="10" t="str">
+        <v/>
+      </c>
+      <c r="R23" s="10" t="str">
+        <v>Feature 3</v>
+      </c>
+      <c r="S23" s="10" t="str">
+        <v>Feature 4</v>
+      </c>
+      <c r="T23" s="10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
@@ -1819,15 +1958,87 @@
       <c r="N24" s="9"/>
       <c r="O24" s="9"/>
     </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="O28" s="11" t="str" cm="1">
+        <f t="array" ref="O28:T30">_xlfn.LAMBDA(_xlpm._s,_xlpm._c,_xlpm._x,_xlpm._p,_xlpm._f,
+_xlfn.LET(
+_xlpm.u,  _xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlpm._s,_xlpm._c="x")),
+_xlpm.ue, _xlfn._xlws.FILTER(_xlpm.u, ISNA(MATCH(_xlpm.u, _exclude, 0))),
+_xlpm.z, _xlfn.HSTACK(_xlpm._s,_xlpm._p,_xlpm._f),
+_xlpm.q, _xlfn.DROP(_xlfn.REDUCE("",_xlpm.ue,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn._xlws.FILTER(_xlpm.z,_xlfn.TAKE(_xlpm.z,,1)=_xlpm.v)))),1),
+_xlfn.PIVOTBY(_xlfn.TAKE(_xlpm.q,,1),_xlfn.CHOOSECOLS(_xlpm.q,2),_xlfn.TAKE(_xlpm.q,,-1),_xlfn.LAMBDA(_xlpm.x,_xlfn.TEXTJOIN(CHAR(10),FALSE,_xlpm.x)),,0,,0)
+))(_tExample[Strategy],_tExample[Critical],_exclude,_tExample[Program],_tExample[Feature])</f>
+        <v/>
+      </c>
+      <c r="P28" s="11" t="str">
+        <v>A</v>
+      </c>
+      <c r="Q28" s="11" t="str">
+        <v>B</v>
+      </c>
+      <c r="R28" s="11" t="str">
+        <v>C</v>
+      </c>
+      <c r="S28" s="11" t="str">
+        <v>D</v>
+      </c>
+      <c r="T28" s="11" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="29" spans="3:20" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="O29" s="10" t="str">
+        <v>Craig</v>
+      </c>
+      <c r="P29" s="10" t="str">
+        <v>Feature 5</v>
+      </c>
+      <c r="Q29" s="10" t="str">
+        <v>Feature 6
+Feature 8</v>
+      </c>
+      <c r="R29" s="10" t="str">
+        <v>Feature 7</v>
+      </c>
+      <c r="S29" s="10" t="str">
+        <v/>
+      </c>
+      <c r="T29" s="10" t="str">
+        <v>Feature 9</v>
+      </c>
+    </row>
+    <row r="30" spans="3:20" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="O30" s="10" t="str">
+        <v>Mark</v>
+      </c>
+      <c r="P30" s="10" t="str">
+        <v>Feature 1
+Feature 2
+Feature A</v>
+      </c>
+      <c r="Q30" s="10" t="str">
+        <v/>
+      </c>
+      <c r="R30" s="10" t="str">
+        <v>Feature 3</v>
+      </c>
+      <c r="S30" s="10" t="str">
+        <v>Feature 4</v>
+      </c>
+      <c r="T30" s="10" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J5:J8">
     <sortCondition ref="J5:J8"/>
   </sortState>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1870,7 +2081,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>17-Jan-2025</v>
+        <v>18-Jan-2025</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -2166,7 +2377,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>17-Jan-2025</v>
+        <v>18-Jan-2025</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>